<commit_message>
Chamaka Ghanam & Jatai files 12/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA58C65-AB69-4333-85C3-10E7BC9164CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D2C4F3-A797-4FD1-9A08-E693B2B69EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4719,9 +4719,9 @@
   <dimension ref="A1:W2010"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A722" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1080" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V1082" sqref="V1082"/>
+      <selection pane="bottomLeft" activeCell="T1086" sqref="T1086"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Raja 4.7 Final Ghana and other edits 13/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D2C4F3-A797-4FD1-9A08-E693B2B69EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04929024-761B-438D-B478-FC6FA63794A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4718,10 +4718,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1080" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1997" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="T1086" sqref="T1086"/>
+      <selection pane="bottomLeft" activeCell="V840" sqref="V840"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Chamaka Ghanam Jatai corrections Tamil - 14/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5D49B7-E687-4EB0-85F4-3AFAE9EE1E72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6550D95-0203-4561-9B7B-4610E08E392E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4718,10 +4718,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1679" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A680" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V840" sqref="V840"/>
+      <selection pane="bottomLeft" activeCell="V687" sqref="V687"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes in Raja output dir 17/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A69C0C1-1AF9-4462-ACF7-F2B5DF088C6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E8DAFD-F2BB-4BA0-A61E-DE4BC3EA06AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4719,9 +4719,9 @@
   <dimension ref="A1:W2010"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1870" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1987" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="T1647" sqref="T1647"/>
+      <selection pane="bottomLeft" activeCell="S2001" sqref="S2001"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>